<commit_message>
fixed logic and added hr
</commit_message>
<xml_diff>
--- a/Team2TM.xlsx
+++ b/Team2TM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soluk\PycharmProjects\NHLfantasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8617635-68E7-4832-8681-55BD66D74052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6734B6B3-F43C-4828-843A-45E55BCC9A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{658D4BAB-4323-490C-8346-87B579F290A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{658D4BAB-4323-490C-8346-87B579F290A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>PHR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="106">
   <si>
     <t>Club</t>
   </si>
@@ -339,6 +333,27 @@
   </si>
   <si>
     <t>Washington Capitals</t>
+  </si>
+  <si>
+    <t>NST</t>
+  </si>
+  <si>
+    <t>L.A</t>
+  </si>
+  <si>
+    <t>N.J</t>
+  </si>
+  <si>
+    <t>S.J</t>
+  </si>
+  <si>
+    <t>T.B</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>HR</t>
   </si>
 </sst>
 </file>
@@ -393,10 +408,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,16 +431,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}" name="Team2TM" displayName="Team2TM" ref="A1:D33" totalsRowShown="0">
-  <autoFilter ref="A1:D33" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}" name="Team2TM" displayName="Team2TM" ref="A1:E33" totalsRowShown="0">
+  <autoFilter ref="A1:E33" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
     <sortCondition ref="B1:B33"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BCE4A142-CCD0-4619-8B19-516D39620180}" name="From"/>
-    <tableColumn id="2" xr3:uid="{A23BE27A-93FF-436D-A1E2-A95C77F61A06}" name="PHR"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{BCE4A142-CCD0-4619-8B19-516D39620180}" name="City"/>
+    <tableColumn id="2" xr3:uid="{A23BE27A-93FF-436D-A1E2-A95C77F61A06}" name="HR"/>
     <tableColumn id="3" xr3:uid="{28159C8A-94F4-4007-9B5B-CD00C4ECE0BA}" name="Club"/>
     <tableColumn id="4" xr3:uid="{65E9311E-9A64-4D30-BB06-D82EB9DE20B5}" name="NHL"/>
+    <tableColumn id="5" xr3:uid="{21422F77-FD27-4DB5-BD80-563292EBAEAE}" name="NST"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -747,476 +764,577 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F084B8F1-68E6-4008-8D24-AEAD63AC6ADE}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="C18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="D21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>65</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B23" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>67</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
         <v>70</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>74</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
         <v>75</v>
       </c>
-      <c r="D25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
         <v>78</v>
       </c>
-      <c r="D26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
         <v>79</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="C28" t="s">
         <v>82</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>83</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="D28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
         <v>85</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>86</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B30" t="s">
         <v>87</v>
       </c>
-      <c r="D29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
         <v>88</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>89</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B31" t="s">
         <v>90</v>
       </c>
-      <c r="D30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
         <v>91</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>92</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>93</v>
       </c>
-      <c r="D31" t="s">
+      <c r="B32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
         <v>95</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>96</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
         <v>97</v>
       </c>
-      <c r="D32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
         <v>98</v>
       </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>100</v>
-      </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="E33" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ag source and misc cleanup
</commit_message>
<xml_diff>
--- a/Team2TM.xlsx
+++ b/Team2TM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soluk\PycharmProjects\NHLfantasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6734B6B3-F43C-4828-843A-45E55BCC9A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB2306-8309-483A-9BCD-8DA2E0CDF5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{658D4BAB-4323-490C-8346-87B579F290A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
   <si>
     <t>Club</t>
   </si>
@@ -354,19 +354,46 @@
   </si>
   <si>
     <t>HR</t>
+  </si>
+  <si>
+    <t>AG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -383,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -404,20 +431,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -431,17 +537,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}" name="Team2TM" displayName="Team2TM" ref="A1:E33" totalsRowShown="0">
-  <autoFilter ref="A1:E33" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}" name="Team2TM" displayName="Team2TM" ref="A1:F33" totalsRowShown="0">
+  <autoFilter ref="A1:F33" xr:uid="{266CDB12-FC32-4C02-B169-32CC16EE103D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
     <sortCondition ref="B1:B33"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BCE4A142-CCD0-4619-8B19-516D39620180}" name="City"/>
     <tableColumn id="2" xr3:uid="{A23BE27A-93FF-436D-A1E2-A95C77F61A06}" name="HR"/>
     <tableColumn id="3" xr3:uid="{28159C8A-94F4-4007-9B5B-CD00C4ECE0BA}" name="Club"/>
     <tableColumn id="4" xr3:uid="{65E9311E-9A64-4D30-BB06-D82EB9DE20B5}" name="NHL"/>
     <tableColumn id="5" xr3:uid="{21422F77-FD27-4DB5-BD80-563292EBAEAE}" name="NST"/>
+    <tableColumn id="6" xr3:uid="{8B698039-A6C7-447F-81A4-EF92D400B86A}" name="AG" dataDxfId="0" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -764,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F084B8F1-68E6-4008-8D24-AEAD63AC6ADE}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +883,7 @@
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -792,8 +899,11 @@
       <c r="E1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -809,8 +919,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -826,8 +939,11 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -843,8 +959,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -860,8 +979,11 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -877,8 +999,11 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -894,8 +1019,11 @@
       <c r="E7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -911,8 +1039,11 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -928,8 +1059,11 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -945,8 +1079,11 @@
       <c r="E10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -962,8 +1099,11 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -979,8 +1119,11 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -996,8 +1139,11 @@
       <c r="E13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1013,8 +1159,11 @@
       <c r="E14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1030,8 +1179,11 @@
       <c r="E15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1047,8 +1199,11 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1064,8 +1219,11 @@
       <c r="E17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1081,8 +1239,11 @@
       <c r="E18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1098,8 +1259,11 @@
       <c r="E19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1115,8 +1279,11 @@
       <c r="E20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1132,8 +1299,11 @@
       <c r="E21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1149,8 +1319,11 @@
       <c r="E22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -1166,8 +1339,11 @@
       <c r="E23" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1183,8 +1359,11 @@
       <c r="E24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1200,8 +1379,11 @@
       <c r="E25" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1217,8 +1399,11 @@
       <c r="E26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1234,8 +1419,11 @@
       <c r="E27" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1251,8 +1439,11 @@
       <c r="E28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1268,8 +1459,11 @@
       <c r="E29" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -1285,8 +1479,11 @@
       <c r="E30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -1302,8 +1499,11 @@
       <c r="E31" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -1319,8 +1519,11 @@
       <c r="E32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1334,6 +1537,9 @@
         <v>97</v>
       </c>
       <c r="E33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>